<commit_message>
Update README.md to enhance terminology section and improve formatting
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -422,7 +422,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,16 +491,8 @@
           <t>22:03:12</t>
         </is>
       </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>Total Duration:</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="inlineStr">
-        <is>
-          <t>0 Hours</t>
-        </is>
-      </c>
+      <c r="C3" s="2" t="n"/>
+      <c r="D3" s="2" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
@@ -511,6 +503,38 @@
       <c r="B4" s="2" t="inlineStr">
         <is>
           <t>22:03:16</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>11:41:38</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>-10.36 Hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-23</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>11:41:51</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>Total Duration:</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>-10.5 Hours</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor diagram in tutorials README to improve clarity and styling of components
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -422,7 +422,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -527,12 +527,38 @@
           <t>11:41:51</t>
         </is>
       </c>
-      <c r="C5" s="2" t="inlineStr">
+      <c r="C5" s="2" t="n"/>
+      <c r="D5" s="2" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-23</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>15:48:02</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>15:48:11</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>0 Hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="C7" s="2" t="inlineStr">
         <is>
           <t>Total Duration:</t>
         </is>
       </c>
-      <c r="D5" s="2" t="inlineStr">
+      <c r="D7" s="2" t="inlineStr">
         <is>
           <t>-10.5 Hours</t>
         </is>

</xml_diff>

<commit_message>
Update terminology and improve clarity in tutorials README
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -553,6 +553,16 @@
       </c>
     </row>
     <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-24</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>22:59:38</t>
+        </is>
+      </c>
       <c r="C7" s="2" t="inlineStr">
         <is>
           <t>Total Duration:</t>

</xml_diff>

<commit_message>
Enhance README with detailed explanation of EventEmitters and provide example usage
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -2,15 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3420" yWindow="3420" windowWidth="16920" windowHeight="10450" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Timesheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -47,7 +46,13 @@
       <diagonal/>
     </border>
     <border>
-      <bottom style="thick"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -59,7 +64,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -422,13 +427,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
     <col width="12" customWidth="1" min="1" max="1"/>
     <col width="17" customWidth="1" min="2" max="2"/>
@@ -436,7 +441,7 @@
     <col width="16" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="15.5" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Date</t>
@@ -458,7 +463,7 @@
         </is>
       </c>
     </row>
-    <row r="2">
+    <row r="2" ht="15.5" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
           <t>2026-01-22</t>
@@ -480,99 +485,47 @@
         </is>
       </c>
     </row>
-    <row r="3">
+    <row r="3" ht="15.5" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>22:03:12</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="n"/>
-      <c r="D3" s="2" t="n"/>
+          <t>15:48:02</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>15:48:11</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>0 Hours</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-25</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>22:03:16</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>11:41:38</t>
-        </is>
-      </c>
-      <c r="D4" s="2" t="inlineStr">
-        <is>
-          <t>-10.36 Hours</t>
+          <t>13:36:27</t>
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>2026-01-23</t>
-        </is>
-      </c>
-      <c r="B5" s="2" t="inlineStr">
-        <is>
-          <t>11:41:51</t>
-        </is>
-      </c>
-      <c r="C5" s="2" t="n"/>
-      <c r="D5" s="2" t="n"/>
+    <row r="5" ht="15.5" customHeight="1">
+      <c r="A5" s="2" t="n"/>
+      <c r="B5" s="2" t="n"/>
     </row>
-    <row r="6">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>2026-01-23</t>
-        </is>
-      </c>
-      <c r="B6" s="2" t="inlineStr">
-        <is>
-          <t>15:48:02</t>
-        </is>
-      </c>
-      <c r="C6" s="2" t="inlineStr">
-        <is>
-          <t>15:48:11</t>
-        </is>
-      </c>
-      <c r="D6" s="2" t="inlineStr">
-        <is>
-          <t>0 Hours</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="inlineStr">
-        <is>
-          <t>2026-01-24</t>
-        </is>
-      </c>
-      <c r="B7" s="2" t="inlineStr">
-        <is>
-          <t>22:59:38</t>
-        </is>
-      </c>
-      <c r="C7" s="2" t="inlineStr">
-        <is>
-          <t>Total Duration:</t>
-        </is>
-      </c>
-      <c r="D7" s="2" t="inlineStr">
-        <is>
-          <t>-10.5 Hours</t>
-        </is>
-      </c>
+    <row r="6" ht="15.5" customHeight="1">
+      <c r="C6" s="2" t="n"/>
+      <c r="D6" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add initial README and enhance index.html with dynamic header creation
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -518,10 +518,38 @@
           <t>13:36:27</t>
         </is>
       </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>18:28:07</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>4.86 Hours</t>
+        </is>
+      </c>
     </row>
     <row r="5" ht="15.5" customHeight="1">
-      <c r="A5" s="2" t="n"/>
-      <c r="B5" s="2" t="n"/>
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>18:58:12</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>Total Duration:</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>5 Hours</t>
+        </is>
+      </c>
     </row>
     <row r="6" ht="15.5" customHeight="1">
       <c r="C6" s="2" t="n"/>

</xml_diff>

<commit_message>
Update timesheet.xlsx with latest entries and adjustments
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -552,6 +552,16 @@
       </c>
     </row>
     <row r="6" ht="15.5" customHeight="1">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>23:19:54</t>
+        </is>
+      </c>
       <c r="C6" s="2" t="n"/>
       <c r="D6" s="2" t="n"/>
     </row>

</xml_diff>

<commit_message>
Update README with company services, add notes for developers, and enhance local testing instructions; add .gitignore files and initial Next.js project structure
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -1,37 +1,86 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kenne\Documents\AborWiseSolutions\ArborWiseSolutions\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B9770A6-D3FA-4CFF-8C9F-AF551C7EE737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3420" yWindow="3420" windowWidth="16920" windowHeight="10450" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Timesheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Timesheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Time Clocked-In</t>
+  </si>
+  <si>
+    <t>Time Clocked-Out</t>
+  </si>
+  <si>
+    <t>Total Duration</t>
+  </si>
+  <si>
+    <t>2026-01-25</t>
+  </si>
+  <si>
+    <t>13:36:27</t>
+  </si>
+  <si>
+    <t>18:28:07</t>
+  </si>
+  <si>
+    <t>4.86 Hours</t>
+  </si>
+  <si>
+    <t>23:19:54</t>
+  </si>
+  <si>
+    <t>23:27:59</t>
+  </si>
+  <si>
+    <t>0.13 Hours</t>
+  </si>
+  <si>
+    <t>Total Duration:</t>
+  </si>
+  <si>
+    <t>5 Hours</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
       <name val="Times New Roman"/>
-      <sz val="12"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -59,82 +108,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -422,149 +412,73 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="12" customWidth="1" min="1" max="1"/>
-    <col width="17" customWidth="1" min="2" max="2"/>
-    <col width="18" customWidth="1" min="3" max="3"/>
-    <col width="16" customWidth="1" min="4" max="4"/>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.5" customHeight="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Time Clocked-In</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Time Clocked-Out</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Total Duration</t>
-        </is>
+    <row r="1" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="2" ht="15.5" customHeight="1">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>2026-01-22</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>22:02:59</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="inlineStr">
-        <is>
-          <t>22:03:06</t>
-        </is>
-      </c>
-      <c r="D2" s="2" t="inlineStr">
-        <is>
-          <t>0 Hours</t>
-        </is>
+    <row r="2" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="3" ht="15.5" customHeight="1">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>2026-01-23</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>15:48:02</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>15:48:11</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="inlineStr">
-        <is>
-          <t>0 Hours</t>
-        </is>
+    <row r="3" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>2026-01-25</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>13:36:27</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>18:28:07</t>
-        </is>
-      </c>
-      <c r="D4" s="2" t="inlineStr">
-        <is>
-          <t>4.86 Hours</t>
-        </is>
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="5" ht="15.5" customHeight="1">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>2026-01-25</t>
-        </is>
-      </c>
-      <c r="B5" s="2" t="inlineStr">
-        <is>
-          <t>18:58:12</t>
-        </is>
-      </c>
-      <c r="C5" s="2" t="inlineStr">
-        <is>
-          <t>Total Duration:</t>
-        </is>
-      </c>
-      <c r="D5" s="2" t="inlineStr">
-        <is>
-          <t>5 Hours</t>
-        </is>
-      </c>
-    </row>
-    <row r="6" ht="15.5" customHeight="1">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>2026-01-25</t>
-        </is>
-      </c>
-      <c r="B6" s="2" t="inlineStr">
-        <is>
-          <t>23:19:54</t>
-        </is>
-      </c>
-      <c r="C6" s="2" t="n"/>
-      <c r="D6" s="2" t="n"/>
-    </row>
+    <row r="5" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Huge file restructure in the `tutorials/next.js project` project folder. Originally there was one `Next.js` project in `tutorials/next.js project` and one `app` file where all the chapters where in `app` past chapter 8. Restructured so now there are two `Next.js` projects in `tutorial/next.js project`. One is in `tutorials/next.js project/react-foundations` and the other is in `tutorials/next.js project/financial-dashboard/nextjs-dashboard`.
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -1,86 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kenne\Documents\AborWiseSolutions\ArborWiseSolutions\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B9770A6-D3FA-4CFF-8C9F-AF551C7EE737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1140" yWindow="1140" windowWidth="16920" windowHeight="10450" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Timesheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Timesheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Time Clocked-In</t>
-  </si>
-  <si>
-    <t>Time Clocked-Out</t>
-  </si>
-  <si>
-    <t>Total Duration</t>
-  </si>
-  <si>
-    <t>2026-01-25</t>
-  </si>
-  <si>
-    <t>13:36:27</t>
-  </si>
-  <si>
-    <t>18:28:07</t>
-  </si>
-  <si>
-    <t>4.86 Hours</t>
-  </si>
-  <si>
-    <t>23:19:54</t>
-  </si>
-  <si>
-    <t>23:27:59</t>
-  </si>
-  <si>
-    <t>0.13 Hours</t>
-  </si>
-  <si>
-    <t>Total Duration:</t>
-  </si>
-  <si>
-    <t>5 Hours</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Times New Roman"/>
       <sz val="12"/>
-      <name val="Times New Roman"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -108,23 +59,82 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -412,73 +422,138 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
+    <col width="12" customWidth="1" min="1" max="1"/>
+    <col width="17" customWidth="1" min="2" max="2"/>
+    <col width="18" customWidth="1" min="3" max="3"/>
+    <col width="16" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
+    <row r="1" ht="15.65" customHeight="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Time Clocked-In</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Time Clocked-Out</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Total Duration</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
+    <row r="2" ht="15.65" customHeight="1">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>13:36:27</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>18:28:07</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>4.86 Hours</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
+    <row r="3" ht="15.65" customHeight="1">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>23:19:54</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>23:27:59</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>0.13 Hours</t>
+        </is>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>12</v>
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-26</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>20:20:26</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>22:25:22</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>2.08 Hours</t>
+        </is>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" ht="15.65" customHeight="1">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-27</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>10:27:48</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>Total Duration:</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>7 Hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="15.65" customHeight="1">
+      <c r="D6" s="2" t="n"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Enhance financial dashboard layout and navigation
- Added global CSS and font imports to layout.
- Updated page structure with responsive design and image handling.
- Implemented client-side navigation with dynamic link highlighting.
- Created new pages for customers and invoices.
- Introduced a shared layout component for consistent UI across dashboard pages.
- Updated font handling for improved typography.
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1140" yWindow="1140" windowWidth="16920" windowHeight="10450" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11175" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Timesheet" sheetId="1" state="visible" r:id="rId1"/>
@@ -427,13 +427,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="12" customWidth="1" min="1" max="1"/>
     <col width="17" customWidth="1" min="2" max="2"/>
@@ -441,7 +441,7 @@
     <col width="16" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.65" customHeight="1">
+    <row r="1" ht="15.6" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Date</t>
@@ -463,7 +463,7 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="15.65" customHeight="1">
+    <row r="2" ht="15.6" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
           <t>2026-01-25</t>
@@ -485,7 +485,7 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="15.65" customHeight="1">
+    <row r="3" ht="15.6" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
           <t>2026-01-25</t>
@@ -529,7 +529,7 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="15.65" customHeight="1">
+    <row r="5" ht="15.6" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
           <t>2026-01-27</t>
@@ -542,17 +542,48 @@
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
+          <t>14:10:45</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>3.71 Hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="15.6" customHeight="1">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-27</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>21:09:12</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
           <t>Total Duration:</t>
         </is>
       </c>
-      <c r="D5" s="2" t="inlineStr">
-        <is>
-          <t>7 Hours</t>
-        </is>
-      </c>
-    </row>
-    <row r="6" ht="15.65" customHeight="1">
-      <c r="D6" s="2" t="n"/>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>14 Hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>22:31:37</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Enhance dashboard with parallel data fetching and updated UI components.
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11175" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2280" yWindow="2280" windowWidth="16920" windowHeight="10450" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Timesheet" sheetId="1" state="visible" r:id="rId1"/>
@@ -430,10 +430,10 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
     <col width="12" customWidth="1" min="1" max="1"/>
     <col width="17" customWidth="1" min="2" max="2"/>
@@ -441,7 +441,7 @@
     <col width="16" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.6" customHeight="1">
+    <row r="1" ht="15.65" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Date</t>
@@ -463,7 +463,7 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="15.6" customHeight="1">
+    <row r="2" ht="15.65" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
           <t>2026-01-25</t>
@@ -485,7 +485,7 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="15.6" customHeight="1">
+    <row r="3" ht="15.65" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
           <t>2026-01-25</t>
@@ -529,7 +529,7 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="15.6" customHeight="1">
+    <row r="5" ht="15.65" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
           <t>2026-01-27</t>
@@ -551,53 +551,55 @@
         </is>
       </c>
     </row>
-    <row r="6" ht="15.6" customHeight="1">
+    <row r="6" ht="15.65" customHeight="1">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>21:09:12</t>
-        </is>
-      </c>
-      <c r="C6" s="2" t="n"/>
-      <c r="D6" s="2" t="n"/>
-    </row>
-    <row r="7">
+          <t>14:58:14</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>15:13:42</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>0.26 Hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="15.5" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>22:31:37</t>
+          <t>16:23:14</t>
         </is>
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>
-          <t>22:22:30</t>
+          <t>Total Duration:</t>
         </is>
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>-0.15 Hours</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="C8" s="2" t="inlineStr">
-        <is>
-          <t>Total Duration:</t>
-        </is>
-      </c>
-      <c r="D8" s="2" t="inlineStr">
-        <is>
-          <t>10.5 Hours</t>
-        </is>
-      </c>
+          <t>11 Hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="15.5" customHeight="1">
+      <c r="A8" s="2" t="n"/>
+      <c r="B8" s="2" t="n"/>
+      <c r="C8" s="2" t="n"/>
+      <c r="D8" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Created API endpoints for project.
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -439,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N22" sqref="N22"/>
@@ -646,16 +646,40 @@
       </c>
     </row>
     <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-02</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>17:53:08</t>
+        </is>
+      </c>
       <c r="C11" s="2" t="inlineStr">
         <is>
-          <t>Total Duration:</t>
+          <t>18:39:28</t>
         </is>
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>-7.5 Hours</t>
-        </is>
-      </c>
+          <t>0.77 Hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-02</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>21:07:41</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="n"/>
+      <c r="D12" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Changes: 1. Fixed Google fonts not loading by editing the `next.config.ts` file. 2. Edited indention in some files. 3. Added a chainsaw `favicon.ico` for our project's tab.
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -63,7 +63,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -73,7 +73,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,10 +438,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -623,7 +622,7 @@
         </is>
       </c>
     </row>
-    <row r="10">
+    <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="2" t="inlineStr">
         <is>
           <t>2026-02-01</t>
@@ -641,11 +640,11 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>-22.91 Hours</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
+          <t>1.08 Hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="2" t="inlineStr">
         <is>
           <t>2026-02-02</t>
@@ -667,7 +666,7 @@
         </is>
       </c>
     </row>
-    <row r="12">
+    <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="2" t="inlineStr">
         <is>
           <t>2026-02-02</t>
@@ -678,8 +677,30 @@
           <t>21:07:41</t>
         </is>
       </c>
-      <c r="C12" s="2" t="n"/>
-      <c r="D12" s="2" t="n"/>
+      <c r="C12" s="2" t="inlineStr">
+        <is>
+          <t>23:03:37</t>
+        </is>
+      </c>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>1.93 Hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="13" ht="15.75" customHeight="1">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="inlineStr">
+        <is>
+          <t>07:59:16</t>
+        </is>
+      </c>
+      <c r="C13" s="2" t="n"/>
+      <c r="D13" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Worked on the header/navigation bar. Added in an SVG for the logo icon. Added in a `<NavigationBar />` component in the `ui/commons` folder.
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
@@ -699,8 +699,52 @@
           <t>07:59:16</t>
         </is>
       </c>
-      <c r="C13" s="2" t="n"/>
-      <c r="D13" s="2" t="n"/>
+      <c r="C13" s="2" t="inlineStr">
+        <is>
+          <t>08:44:48</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>0.76 Hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="inlineStr">
+        <is>
+          <t>12:52:45</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="inlineStr">
+        <is>
+          <t>13:01:55</t>
+        </is>
+      </c>
+      <c r="D14" s="2" t="inlineStr">
+        <is>
+          <t>0.15 Hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>16:15:23</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="n"/>
+      <c r="D15" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Changes: 1. Removed content from `page.tsx` in the `app` folder (the home page) besides the basic HTML skeleton. 2. Worked on the `<NavigationBar />` component.
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
@@ -743,8 +743,52 @@
           <t>16:15:23</t>
         </is>
       </c>
-      <c r="C15" s="2" t="n"/>
-      <c r="D15" s="2" t="n"/>
+      <c r="C15" s="2" t="inlineStr">
+        <is>
+          <t>18:49:35</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="inlineStr">
+        <is>
+          <t>2.57 Hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="inlineStr">
+        <is>
+          <t>20:26:35</t>
+        </is>
+      </c>
+      <c r="C16" s="2" t="inlineStr">
+        <is>
+          <t>21:25:16</t>
+        </is>
+      </c>
+      <c r="D16" s="2" t="inlineStr">
+        <is>
+          <t>0.98 Hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="inlineStr">
+        <is>
+          <t>21:32:50</t>
+        </is>
+      </c>
+      <c r="C17" s="2" t="n"/>
+      <c r="D17" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Updated the Tailwind CSS of the `<NavigationBar />` component's elements to format correctly and also added a revving chainsaw using Sora to the homepage component.
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
@@ -787,8 +787,50 @@
           <t>21:32:50</t>
         </is>
       </c>
-      <c r="C17" s="2" t="n"/>
-      <c r="D17" s="2" t="n"/>
+      <c r="C17" s="2" t="inlineStr">
+        <is>
+          <t>23:14:51</t>
+        </is>
+      </c>
+      <c r="D17" s="2" t="inlineStr">
+        <is>
+          <t>1.7 Hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="inlineStr">
+        <is>
+          <t>00:06:07</t>
+        </is>
+      </c>
+      <c r="C18" s="2" t="inlineStr">
+        <is>
+          <t>00:06:10</t>
+        </is>
+      </c>
+      <c r="D18" s="2" t="inlineStr">
+        <is>
+          <t>0 Hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="C19" s="2" t="inlineStr">
+        <is>
+          <t>Total Duration:</t>
+        </is>
+      </c>
+      <c r="D19" s="2" t="inlineStr">
+        <is>
+          <t>25.5 Hours</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added hero icons to the `<NavigationBar />` component.
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -821,16 +821,18 @@
       </c>
     </row>
     <row r="19">
-      <c r="C19" s="2" t="inlineStr">
-        <is>
-          <t>Total Duration:</t>
-        </is>
-      </c>
-      <c r="D19" s="2" t="inlineStr">
-        <is>
-          <t>25.5 Hours</t>
-        </is>
-      </c>
+      <c r="A19" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-05</t>
+        </is>
+      </c>
+      <c r="B19" s="2" t="inlineStr">
+        <is>
+          <t>21:38:36</t>
+        </is>
+      </c>
+      <c r="C19" s="2" t="n"/>
+      <c r="D19" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added two more components in the folder `ui/common/navigation`. One component for desktop links and one component for mobile links to make more responsive `<NavigationBar />`.
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
@@ -831,8 +831,28 @@
           <t>21:38:36</t>
         </is>
       </c>
-      <c r="C19" s="2" t="n"/>
-      <c r="D19" s="2" t="n"/>
+      <c r="C19" s="2" t="inlineStr">
+        <is>
+          <t>22:37:50</t>
+        </is>
+      </c>
+      <c r="D19" s="2" t="inlineStr">
+        <is>
+          <t>0.99 Hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="C20" s="2" t="inlineStr">
+        <is>
+          <t>Total Duration:</t>
+        </is>
+      </c>
+      <c r="D20" s="2" t="inlineStr">
+        <is>
+          <t>26.5 Hours</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Generated an SVG for the hero video in the background on home page.
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
@@ -843,14 +843,58 @@
       </c>
     </row>
     <row r="20">
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-06</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="inlineStr">
+        <is>
+          <t>16:57:32</t>
+        </is>
+      </c>
       <c r="C20" s="2" t="inlineStr">
         <is>
+          <t>18:11:58</t>
+        </is>
+      </c>
+      <c r="D20" s="2" t="inlineStr">
+        <is>
+          <t>1.24 Hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-06</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="inlineStr">
+        <is>
+          <t>19:15:30</t>
+        </is>
+      </c>
+      <c r="C21" s="2" t="inlineStr">
+        <is>
+          <t>19:43:57</t>
+        </is>
+      </c>
+      <c r="D21" s="2" t="inlineStr">
+        <is>
+          <t>0.47 Hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="C22" s="2" t="inlineStr">
+        <is>
           <t>Total Duration:</t>
         </is>
       </c>
-      <c r="D20" s="2" t="inlineStr">
-        <is>
-          <t>26.5 Hours</t>
+      <c r="D22" s="2" t="inlineStr">
+        <is>
+          <t>28 Hours</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Adjusted the `<NavigationBar />` component to use fixed tailwind CSS heights.
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -887,16 +887,18 @@
       </c>
     </row>
     <row r="22">
-      <c r="C22" s="2" t="inlineStr">
-        <is>
-          <t>Total Duration:</t>
-        </is>
-      </c>
-      <c r="D22" s="2" t="inlineStr">
-        <is>
-          <t>28 Hours</t>
-        </is>
-      </c>
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-07</t>
+        </is>
+      </c>
+      <c r="B22" s="2" t="inlineStr">
+        <is>
+          <t>12:30:38</t>
+        </is>
+      </c>
+      <c r="C22" s="2" t="n"/>
+      <c r="D22" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Refactor NavigationBar to include MobileNav component and adjust header height; update hero section height calculation in page.tsx
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
@@ -897,8 +897,50 @@
           <t>12:30:38</t>
         </is>
       </c>
-      <c r="C22" s="2" t="n"/>
-      <c r="D22" s="2" t="n"/>
+      <c r="C22" s="2" t="inlineStr">
+        <is>
+          <t>12:59:28</t>
+        </is>
+      </c>
+      <c r="D22" s="2" t="inlineStr">
+        <is>
+          <t>0.48 Hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-07</t>
+        </is>
+      </c>
+      <c r="B23" s="2" t="inlineStr">
+        <is>
+          <t>13:12:53</t>
+        </is>
+      </c>
+      <c r="C23" s="2" t="inlineStr">
+        <is>
+          <t>13:40:48</t>
+        </is>
+      </c>
+      <c r="D23" s="2" t="inlineStr">
+        <is>
+          <t>0.47 Hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="C24" s="2" t="inlineStr">
+        <is>
+          <t>Total Duration:</t>
+        </is>
+      </c>
+      <c r="D24" s="2" t="inlineStr">
+        <is>
+          <t>29 Hours</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Refactored the home page/screen.
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
@@ -931,14 +931,58 @@
       </c>
     </row>
     <row r="24">
+      <c r="A24" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-12</t>
+        </is>
+      </c>
+      <c r="B24" s="2" t="inlineStr">
+        <is>
+          <t>20:45:46</t>
+        </is>
+      </c>
       <c r="C24" s="2" t="inlineStr">
         <is>
+          <t>21:04:21</t>
+        </is>
+      </c>
+      <c r="D24" s="2" t="inlineStr">
+        <is>
+          <t>0.31 Hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-15</t>
+        </is>
+      </c>
+      <c r="B25" s="2" t="inlineStr">
+        <is>
+          <t>17:02:42</t>
+        </is>
+      </c>
+      <c r="C25" s="2" t="inlineStr">
+        <is>
+          <t>17:57:29</t>
+        </is>
+      </c>
+      <c r="D25" s="2" t="inlineStr">
+        <is>
+          <t>0.91 Hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="C26" s="2" t="inlineStr">
+        <is>
           <t>Total Duration:</t>
         </is>
       </c>
-      <c r="D24" s="2" t="inlineStr">
-        <is>
-          <t>29 Hours</t>
+      <c r="D26" s="2" t="inlineStr">
+        <is>
+          <t>30 Hours</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update typography styles in globals.css and enhance hero section in page.tsx; add new text.txt file
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
@@ -975,16 +975,40 @@
       </c>
     </row>
     <row r="26">
+      <c r="A26" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-16</t>
+        </is>
+      </c>
+      <c r="B26" s="2" t="inlineStr">
+        <is>
+          <t>14:00:34</t>
+        </is>
+      </c>
       <c r="C26" s="2" t="inlineStr">
         <is>
-          <t>Total Duration:</t>
+          <t>14:36:07</t>
         </is>
       </c>
       <c r="D26" s="2" t="inlineStr">
         <is>
-          <t>30 Hours</t>
-        </is>
-      </c>
+          <t>0.59 Hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-16</t>
+        </is>
+      </c>
+      <c r="B27" s="2" t="inlineStr">
+        <is>
+          <t>15:29:20</t>
+        </is>
+      </c>
+      <c r="C27" s="2" t="n"/>
+      <c r="D27" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add service process SVG diagram with detailed steps and icons
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
@@ -1019,14 +1019,36 @@
       </c>
     </row>
     <row r="28">
+      <c r="A28" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-16</t>
+        </is>
+      </c>
+      <c r="B28" s="2" t="inlineStr">
+        <is>
+          <t>22:22:03</t>
+        </is>
+      </c>
       <c r="C28" s="2" t="inlineStr">
         <is>
+          <t>23:22:45</t>
+        </is>
+      </c>
+      <c r="D28" s="2" t="inlineStr">
+        <is>
+          <t>1.01 Hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="C29" s="2" t="inlineStr">
+        <is>
           <t>Total Duration:</t>
         </is>
       </c>
-      <c r="D28" s="2" t="inlineStr">
-        <is>
-          <t>32 Hours</t>
+      <c r="D29" s="2" t="inlineStr">
+        <is>
+          <t>33 Hours</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added a chainsaw model on the homepage.
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
@@ -1041,14 +1041,36 @@
       </c>
     </row>
     <row r="29">
+      <c r="A29" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-18</t>
+        </is>
+      </c>
+      <c r="B29" s="2" t="inlineStr">
+        <is>
+          <t>23:12:52</t>
+        </is>
+      </c>
       <c r="C29" s="2" t="inlineStr">
         <is>
+          <t>23:55:46</t>
+        </is>
+      </c>
+      <c r="D29" s="2" t="inlineStr">
+        <is>
+          <t>0.71 Hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="C30" s="2" t="inlineStr">
+        <is>
           <t>Total Duration:</t>
         </is>
       </c>
-      <c r="D29" s="2" t="inlineStr">
-        <is>
-          <t>33 Hours</t>
+      <c r="D30" s="2" t="inlineStr">
+        <is>
+          <t>33.5 Hours</t>
         </is>
       </c>
     </row>

</xml_diff>